<commit_message>
Fix social service name
</commit_message>
<xml_diff>
--- a/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
+++ b/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/code/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/activities/social_services/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A194C7-6732-4F49-BC9D-10DC3A25C81C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4095"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">גיליון1!$B$2:$F$59</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,9 +77,6 @@
     <t>הפעלת מרכזים למזעור נזקים למשתמשי סמים</t>
   </si>
   <si>
-    <t xml:space="preserve">  'ביצוע בדיקת זכאות לנכות על פי חוק השיקום</t>
-  </si>
-  <si>
     <t>רכישת שירותי הפעלה וקיום תכנית "אוניברסיטה בעם"</t>
   </si>
   <si>
@@ -296,21 +309,24 @@
   </si>
   <si>
     <t>מיקום מדדים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ביצוע בדיקת זכאות לנכות על פי חוק השיקום</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -318,7 +334,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -327,7 +343,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -335,21 +351,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -357,7 +373,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -365,21 +381,21 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -387,14 +403,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -565,7 +581,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -610,16 +626,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -628,7 +644,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,7 +653,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,7 +662,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -656,7 +672,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -703,7 +719,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -745,7 +761,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -778,9 +794,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,6 +846,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -988,32 +1038,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="24.375" style="5" customWidth="1"/>
-    <col min="7" max="9" width="8.625" style="2"/>
-    <col min="10" max="11" width="12.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.625" style="2"/>
+    <col min="1" max="1" width="4.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="5" customWidth="1"/>
+    <col min="7" max="9" width="8.6640625" style="2"/>
+    <col min="10" max="11" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H1" s="40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>0</v>
@@ -1031,51 +1081,51 @@
         <v>4</v>
       </c>
       <c r="G2" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="I2" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="P2" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="19">
         <v>2140000</v>
@@ -1084,14 +1134,14 @@
         <v>13600</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="44"/>
       <c r="D4" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="19">
         <v>36800</v>
@@ -1100,14 +1150,14 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="42"/>
       <c r="C5" s="44"/>
       <c r="D5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="19">
         <v>4000</v>
@@ -1116,14 +1166,14 @@
         <v>24096</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="45"/>
       <c r="D6" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="19">
         <v>1200</v>
@@ -1132,12 +1182,12 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="25" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="42"/>
       <c r="C7" s="22"/>
       <c r="D7" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="24">
         <f>SUM(E3:E6)</f>
@@ -1145,7 +1195,7 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -1154,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="20">
         <v>235621</v>
@@ -1163,14 +1213,14 @@
         <v>3665</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>6</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="44"/>
       <c r="D9" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="20">
         <v>235621</v>
@@ -1179,14 +1229,14 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>7</v>
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="44"/>
       <c r="D10" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="20">
         <v>200000.003</v>
@@ -1196,14 +1246,14 @@
       </c>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>8</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="44"/>
       <c r="D11" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="20">
         <v>170485</v>
@@ -1213,14 +1263,14 @@
       </c>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>9</v>
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="44"/>
       <c r="D12" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="20">
         <v>169222</v>
@@ -1229,14 +1279,14 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>10</v>
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="20">
         <v>130000</v>
@@ -1245,14 +1295,14 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>11</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="44"/>
       <c r="D14" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="20">
         <v>120000</v>
@@ -1261,14 +1311,14 @@
         <v>10577</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>12</v>
       </c>
       <c r="B15" s="42"/>
       <c r="C15" s="44"/>
       <c r="D15" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="20">
         <v>83000</v>
@@ -1277,14 +1327,14 @@
         <v>6732</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>13</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="44"/>
       <c r="D16" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="20">
         <v>78000</v>
@@ -1293,14 +1343,14 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>14</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="44"/>
       <c r="D17" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="20">
         <v>33000</v>
@@ -1309,14 +1359,14 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>15</v>
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="44"/>
       <c r="D18" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="20">
         <v>30000</v>
@@ -1325,14 +1375,14 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>16</v>
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="44"/>
       <c r="D19" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="20">
         <v>20000</v>
@@ -1341,14 +1391,14 @@
         <v>800</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="40" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>17</v>
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="44"/>
       <c r="D20" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="20">
         <v>19500</v>
@@ -1357,14 +1407,14 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="40" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>18</v>
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="44"/>
       <c r="D21" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="20">
         <v>13000</v>
@@ -1373,14 +1423,14 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>19</v>
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="44"/>
       <c r="D22" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="20">
         <v>12000</v>
@@ -1389,14 +1439,14 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>20</v>
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="44"/>
       <c r="D23" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="20">
         <v>8700</v>
@@ -1405,14 +1455,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="40" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>21</v>
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="44"/>
       <c r="D24" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="20">
         <v>8700</v>
@@ -1421,14 +1471,14 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>22</v>
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="44"/>
       <c r="D25" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="20">
         <v>7500</v>
@@ -1437,14 +1487,14 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>23</v>
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="44"/>
       <c r="D26" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="20">
         <v>7375</v>
@@ -1453,14 +1503,14 @@
         <v>7473</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>24</v>
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="44"/>
       <c r="D27" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="20">
         <v>5500</v>
@@ -1469,14 +1519,14 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="40" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>25</v>
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="44"/>
       <c r="D28" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" s="20">
         <v>3500</v>
@@ -1485,14 +1535,14 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>26</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="44"/>
       <c r="D29" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="20">
         <v>1500</v>
@@ -1501,14 +1551,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>27</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="44"/>
       <c r="D30" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" s="20">
         <v>1200</v>
@@ -1518,14 +1568,14 @@
       </c>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>28</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="44"/>
       <c r="D31" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="20">
         <v>1087.5999999999999</v>
@@ -1535,14 +1585,14 @@
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="54" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>29</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="44"/>
       <c r="D32" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="20">
         <v>730</v>
@@ -1552,14 +1602,14 @@
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>30</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="44"/>
       <c r="D33" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" s="20">
         <v>680</v>
@@ -1568,14 +1618,14 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>31</v>
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="44"/>
       <c r="D34" s="15" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="E34" s="20">
         <v>650</v>
@@ -1584,7 +1634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>32</v>
       </c>
@@ -1600,16 +1650,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>33</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E36" s="20">
         <v>50000</v>
@@ -1618,14 +1668,14 @@
         <v>400</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>34</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="44"/>
       <c r="D37" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E37" s="20">
         <v>18146</v>
@@ -1634,14 +1684,14 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>35</v>
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="44"/>
       <c r="D38" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E38" s="20">
         <v>2200</v>
@@ -1650,14 +1700,14 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>36</v>
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="45"/>
       <c r="D39" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="20">
         <v>350</v>
@@ -1666,7 +1716,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>37</v>
       </c>
@@ -1675,7 +1725,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E40" s="20">
         <v>12500</v>
@@ -1684,14 +1734,14 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>38</v>
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="44"/>
       <c r="D41" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="20">
         <v>9600</v>
@@ -1700,14 +1750,14 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>39</v>
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="44"/>
       <c r="D42" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E42" s="20">
         <v>4000</v>
@@ -1716,14 +1766,14 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>40</v>
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="44"/>
       <c r="D43" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E43" s="20">
         <v>4000</v>
@@ -1732,7 +1782,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>41</v>
       </c>
@@ -1748,7 +1798,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>42</v>
       </c>
@@ -1764,16 +1814,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>43</v>
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E46" s="20">
         <v>3620</v>
@@ -1782,14 +1832,14 @@
         <v>6951</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>44</v>
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="44"/>
       <c r="D47" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E47" s="20">
         <v>2000</v>
@@ -1798,14 +1848,14 @@
         <v>714</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>45</v>
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="44"/>
       <c r="D48" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E48" s="20">
         <v>1146</v>
@@ -1814,7 +1864,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>46</v>
       </c>
@@ -1830,32 +1880,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>47</v>
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E50" s="20">
         <v>5000</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>48</v>
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="45"/>
       <c r="D51" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" s="20">
         <v>1000</v>
@@ -1864,30 +1914,30 @@
         <v>20638</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>49</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="E52" s="20">
         <v>3870</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="16"/>
       <c r="C53" s="26"/>
       <c r="D53" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" s="27">
         <f>SUM(E8:E52)</f>
@@ -1895,18 +1945,18 @@
       </c>
       <c r="F53" s="28"/>
     </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>50</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>57</v>
       </c>
       <c r="E54" s="20">
         <v>100000</v>
@@ -1915,16 +1965,16 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>51</v>
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E55" s="20">
         <v>80237</v>
@@ -1933,16 +1983,16 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>52</v>
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="E56" s="20">
         <v>3000</v>
@@ -1951,25 +2001,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>53</v>
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E57" s="20">
         <v>1500</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>54</v>
       </c>
@@ -1987,11 +2037,11 @@
         <v>752</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="36" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" s="36" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="B59" s="42"/>
       <c r="C59" s="22"/>
       <c r="D59" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E59" s="30">
         <f>SUM(E54:E58)</f>
@@ -1999,11 +2049,11 @@
       </c>
       <c r="F59" s="31"/>
     </row>
-    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" ht="26" x14ac:dyDescent="0.3">
       <c r="B60" s="32"/>
       <c r="C60" s="33"/>
       <c r="D60" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E60" s="34">
         <f>SUM(E59,E53,E7)</f>
@@ -2012,7 +2062,7 @@
       <c r="F60" s="35"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F59"/>
+  <autoFilter ref="B2:F59" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="8">
     <mergeCell ref="B3:B51"/>
     <mergeCell ref="B54:B59"/>

</xml_diff>

<commit_message>
Harmonize service names (1)
</commit_message>
<xml_diff>
--- a/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
+++ b/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/code/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/activities/social_services/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Code/obudget/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/activities/social_services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A194C7-6732-4F49-BC9D-10DC3A25C81C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80634FC7-DC58-034A-A8A6-FAB63D4EACAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -209,9 +209,6 @@
     <t>שיקום נכי נפש בקהילה- תעסוקה - מפעל מוגן</t>
   </si>
   <si>
-    <t xml:space="preserve">מכשירי שיקום וניידות- התאמה, תיקון וחלוקת מכשירי שיקום וניידות </t>
-  </si>
-  <si>
     <t>שיקום נכי נפש בקהילה- חברה - חונכות אקדמית</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t xml:space="preserve">  ביצוע בדיקת זכאות לנכות על פי חוק השיקום</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מכשירי שיקום וניידות – אספקה, התאמה, תיקון וחלוקת מכשירי שיקום וניידות </t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1060,7 +1060,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H1" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
@@ -1081,37 +1081,37 @@
         <v>4</v>
       </c>
       <c r="G2" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="I2" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="P2" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="39" t="s">
         <v>89</v>
-      </c>
-      <c r="Q2" s="39" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -1119,13 +1119,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="19">
         <v>2140000</v>
@@ -1173,7 +1173,7 @@
       <c r="B6" s="42"/>
       <c r="C6" s="45"/>
       <c r="D6" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="19">
         <v>1200</v>
@@ -1187,7 +1187,7 @@
       <c r="B7" s="42"/>
       <c r="C7" s="22"/>
       <c r="D7" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="24">
         <f>SUM(E3:E6)</f>
@@ -1204,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="20">
         <v>235621</v>
@@ -1220,7 +1220,7 @@
       <c r="B9" s="42"/>
       <c r="C9" s="44"/>
       <c r="D9" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="20">
         <v>235621</v>
@@ -1236,7 +1236,7 @@
       <c r="B10" s="42"/>
       <c r="C10" s="44"/>
       <c r="D10" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="20">
         <v>200000.003</v>
@@ -1253,7 +1253,7 @@
       <c r="B11" s="42"/>
       <c r="C11" s="44"/>
       <c r="D11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="20">
         <v>170485</v>
@@ -1270,7 +1270,7 @@
       <c r="B12" s="42"/>
       <c r="C12" s="44"/>
       <c r="D12" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="20">
         <v>169222</v>
@@ -1279,14 +1279,14 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>10</v>
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E13" s="20">
         <v>130000</v>
@@ -1625,7 +1625,7 @@
       <c r="B34" s="42"/>
       <c r="C34" s="44"/>
       <c r="D34" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E34" s="20">
         <v>650</v>
@@ -1659,7 +1659,7 @@
         <v>25</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E36" s="20">
         <v>50000</v>
@@ -1675,7 +1675,7 @@
       <c r="B37" s="42"/>
       <c r="C37" s="44"/>
       <c r="D37" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" s="20">
         <v>18146</v>
@@ -1707,7 +1707,7 @@
       <c r="B39" s="42"/>
       <c r="C39" s="45"/>
       <c r="D39" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E39" s="20">
         <v>350</v>
@@ -1895,7 +1895,7 @@
         <v>5000</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>3870</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
       <c r="B53" s="16"/>
       <c r="C53" s="26"/>
       <c r="D53" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E53" s="27">
         <f>SUM(E8:E52)</f>
@@ -1950,7 +1950,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>55</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>53</v>
@@ -2010,13 +2010,13 @@
         <v>23</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E57" s="20">
         <v>1500</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
       <c r="B59" s="42"/>
       <c r="C59" s="22"/>
       <c r="D59" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E59" s="30">
         <f>SUM(E54:E58)</f>
@@ -2053,7 +2053,7 @@
       <c r="B60" s="32"/>
       <c r="C60" s="33"/>
       <c r="D60" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E60" s="34">
         <f>SUM(E59,E53,E7)</f>

</xml_diff>

<commit_message>
Harmonize service names (2)
</commit_message>
<xml_diff>
--- a/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
+++ b/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Code/obudget/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/activities/social_services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80634FC7-DC58-034A-A8A6-FAB63D4EACAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9009145F-0844-7C44-876D-8E1D8A84864D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,9 +221,6 @@
     <t>תחליפי אשפוז -טיפול בבעלי תחלואה כפולה</t>
   </si>
   <si>
-    <t>שיקום נכי נפש בקהילה- דיור - הוסטלים</t>
-  </si>
-  <si>
     <t>תיקונים של מכשירי ניידות ממונעים</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t xml:space="preserve">מכשירי שיקום וניידות – אספקה, התאמה, תיקון וחלוקת מכשירי שיקום וניידות </t>
+  </si>
+  <si>
+    <t xml:space="preserve">שיקום נכי נפש בקהילה- שירותי שיקום בדיור (הוסטלים) </t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1060,7 +1060,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H1" s="40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
@@ -1081,37 +1081,37 @@
         <v>4</v>
       </c>
       <c r="G2" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="I2" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="P2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="39" t="s">
         <v>88</v>
-      </c>
-      <c r="Q2" s="39" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -1119,13 +1119,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="19">
         <v>2140000</v>
@@ -1173,7 +1173,7 @@
       <c r="B6" s="42"/>
       <c r="C6" s="45"/>
       <c r="D6" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="19">
         <v>1200</v>
@@ -1187,7 +1187,7 @@
       <c r="B7" s="42"/>
       <c r="C7" s="22"/>
       <c r="D7" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="24">
         <f>SUM(E3:E6)</f>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="E8" s="20">
         <v>235621</v>
@@ -1279,14 +1279,14 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>10</v>
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="20">
         <v>130000</v>
@@ -1625,7 +1625,7 @@
       <c r="B34" s="42"/>
       <c r="C34" s="44"/>
       <c r="D34" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E34" s="20">
         <v>650</v>
@@ -1659,7 +1659,7 @@
         <v>25</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" s="20">
         <v>50000</v>
@@ -1675,7 +1675,7 @@
       <c r="B37" s="42"/>
       <c r="C37" s="44"/>
       <c r="D37" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E37" s="20">
         <v>18146</v>
@@ -1707,7 +1707,7 @@
       <c r="B39" s="42"/>
       <c r="C39" s="45"/>
       <c r="D39" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E39" s="20">
         <v>350</v>
@@ -1895,7 +1895,7 @@
         <v>5000</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>3870</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
       <c r="B53" s="16"/>
       <c r="C53" s="26"/>
       <c r="D53" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E53" s="27">
         <f>SUM(E8:E52)</f>
@@ -1950,7 +1950,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>55</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>53</v>
@@ -2010,13 +2010,13 @@
         <v>23</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E57" s="20">
         <v>1500</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
       <c r="B59" s="42"/>
       <c r="C59" s="22"/>
       <c r="D59" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" s="30">
         <f>SUM(E54:E58)</f>
@@ -2053,7 +2053,7 @@
       <c r="B60" s="32"/>
       <c r="C60" s="33"/>
       <c r="D60" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E60" s="34">
         <f>SUM(E59,E53,E7)</f>

</xml_diff>

<commit_message>
Connect activities to budget items
</commit_message>
<xml_diff>
--- a/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
+++ b/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתים בריאות 2016.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Code/obudget/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/activities/social_services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9009145F-0844-7C44-876D-8E1D8A84864D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77123E55-C470-D549-93D2-74E245C304A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>שיקום נכי נפש בקהילה- חברה - מועדונים חברתיים</t>
   </si>
   <si>
-    <t>אשפוזיות- שירותי גמילה</t>
-  </si>
-  <si>
     <t>תחליפי אשפוז -טיפול בבעלי תחלואה כפולה</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t xml:space="preserve">שיקום נכי נפש בקהילה- שירותי שיקום בדיור (הוסטלים) </t>
+  </si>
+  <si>
+    <t>אשפוזיות גמילה מסמים, אלכוהול וחומרים פסיכואקטיביים</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1060,7 +1060,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H1" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
@@ -1081,37 +1081,37 @@
         <v>4</v>
       </c>
       <c r="G2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="I2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="P2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="39" t="s">
         <v>87</v>
-      </c>
-      <c r="Q2" s="39" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="20" x14ac:dyDescent="0.25">
@@ -1119,13 +1119,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="19">
         <v>2140000</v>
@@ -1173,7 +1173,7 @@
       <c r="B6" s="42"/>
       <c r="C6" s="45"/>
       <c r="D6" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="19">
         <v>1200</v>
@@ -1187,7 +1187,7 @@
       <c r="B7" s="42"/>
       <c r="C7" s="22"/>
       <c r="D7" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" s="24">
         <f>SUM(E3:E6)</f>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="20">
         <v>235621</v>
@@ -1220,7 +1220,7 @@
       <c r="B9" s="42"/>
       <c r="C9" s="44"/>
       <c r="D9" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="20">
         <v>235621</v>
@@ -1229,14 +1229,14 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>7</v>
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="44"/>
       <c r="D10" s="13" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="E10" s="20">
         <v>200000.003</v>
@@ -1286,7 +1286,7 @@
       <c r="B13" s="42"/>
       <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="20">
         <v>130000</v>
@@ -1625,7 +1625,7 @@
       <c r="B34" s="42"/>
       <c r="C34" s="44"/>
       <c r="D34" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="20">
         <v>650</v>
@@ -1659,7 +1659,7 @@
         <v>25</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="20">
         <v>50000</v>
@@ -1675,7 +1675,7 @@
       <c r="B37" s="42"/>
       <c r="C37" s="44"/>
       <c r="D37" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E37" s="20">
         <v>18146</v>
@@ -1707,7 +1707,7 @@
       <c r="B39" s="42"/>
       <c r="C39" s="45"/>
       <c r="D39" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E39" s="20">
         <v>350</v>
@@ -1895,7 +1895,7 @@
         <v>5000</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>3870</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
       <c r="B53" s="16"/>
       <c r="C53" s="26"/>
       <c r="D53" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E53" s="27">
         <f>SUM(E8:E52)</f>
@@ -1950,7 +1950,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>55</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>53</v>
@@ -2010,13 +2010,13 @@
         <v>23</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E57" s="20">
         <v>1500</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
       <c r="B59" s="42"/>
       <c r="C59" s="22"/>
       <c r="D59" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E59" s="30">
         <f>SUM(E54:E58)</f>
@@ -2053,7 +2053,7 @@
       <c r="B60" s="32"/>
       <c r="C60" s="33"/>
       <c r="D60" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E60" s="34">
         <f>SUM(E59,E53,E7)</f>

</xml_diff>